<commit_message>
Prohibition Integration into Verification
</commit_message>
<xml_diff>
--- a/src/main/java/POMA/PolicyGeneration/GPMS_Colleges.xlsx
+++ b/src/main/java/POMA/PolicyGeneration/GPMS_Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dubro\git\POMA\src\main\java\POMA\PolicyGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8DF2D1-8E7E-4938-A62E-504D6D1BAF8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D417289-CBE7-4B04-9289-F68C559B629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2970" windowWidth="21600" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17295" yWindow="6120" windowWidth="21600" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>ECON(Economics)</t>
   </si>
   <si>
-    <t>MATH</t>
-  </si>
-  <si>
-    <t>CIV(Civil Engineering)</t>
-  </si>
-  <si>
     <t>MEC(Mechanical Engineering)</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>EDU(EDUCATION)</t>
   </si>
   <si>
-    <t>EARLY(Early childhood)</t>
-  </si>
-  <si>
     <t>ELEM(Elementary School)</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>BA(Business Administration)</t>
   </si>
   <si>
-    <t>ACC(Accountiong)</t>
-  </si>
-  <si>
     <t>FIN(Finance)</t>
   </si>
   <si>
@@ -133,13 +121,25 @@
   </si>
   <si>
     <t>NURS(Nursing)</t>
+  </si>
+  <si>
+    <t>CE(Computer Engineering)</t>
+  </si>
+  <si>
+    <t>MATH(Mathematics)</t>
+  </si>
+  <si>
+    <t>EARLY(Early Childhood)</t>
+  </si>
+  <si>
+    <t>ACC(Accounting)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -203,6 +209,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,13 +522,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -553,73 +562,73 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
+      <c r="A4" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>